<commit_message>
Kannst du das lesen?
</commit_message>
<xml_diff>
--- a/proj1/outputfiles/output.xlsx
+++ b/proj1/outputfiles/output.xlsx
@@ -454,19 +454,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.0001201629638671875</v>
       </c>
       <c r="D2">
-        <v>0.5050847457627119</v>
+        <v>0.4169491525423729</v>
       </c>
       <c r="E2">
         <v>290</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.0001289844512939453</v>
       </c>
       <c r="G2">
         <v>0.9830508474576272</v>
@@ -480,19 +480,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>720</v>
+        <v>679</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.0001001358032226562</v>
       </c>
       <c r="D3">
-        <v>0.703125</v>
+        <v>0.6630859375</v>
       </c>
       <c r="E3">
         <v>1018</v>
       </c>
       <c r="F3">
-        <v>0.0009768009185791016</v>
+        <v>0.0002388954162597656</v>
       </c>
       <c r="G3">
         <v>0.994140625</v>
@@ -506,19 +506,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>4.982948303222656E-05</v>
       </c>
       <c r="D4">
-        <v>0.6857142857142857</v>
+        <v>0.9428571428571428</v>
       </c>
       <c r="E4">
         <v>35</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>3.194808959960938E-05</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -535,7 +535,7 @@
         <v>22</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>5.292892456054688E-05</v>
       </c>
       <c r="D5">
         <v>0.9565217391304348</v>
@@ -544,7 +544,7 @@
         <v>16</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>5.292892456054688E-05</v>
       </c>
       <c r="G5">
         <v>0.6956521739130435</v>
@@ -558,19 +558,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.0001249313354492188</v>
       </c>
       <c r="D6">
-        <v>0.8269230769230769</v>
+        <v>0.8076923076923077</v>
       </c>
       <c r="E6">
         <v>52</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>6.580352783203125E-05</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -584,19 +584,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="C7">
-        <v>0.0009944438934326172</v>
+        <v>3.814697265625E-05</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.7383177570093458</v>
       </c>
       <c r="E7">
         <v>90</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.0003659725189208984</v>
       </c>
       <c r="G7">
         <v>0.8411214953271028</v>
@@ -610,19 +610,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>9619</v>
+        <v>9588</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>7.605552673339844E-05</v>
       </c>
       <c r="D8">
-        <v>0.9848469335517559</v>
+        <v>0.9816729804443535</v>
       </c>
       <c r="E8">
         <v>9753</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.0002660751342773438</v>
       </c>
       <c r="G8">
         <v>0.9985666018224634</v>
@@ -639,7 +639,7 @@
         <v>118</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>3.314018249511719E-05</v>
       </c>
       <c r="D9">
         <v>0.9076923076923077</v>
@@ -648,7 +648,7 @@
         <v>130</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>8.511543273925781E-05</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -662,19 +662,19 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>687</v>
+        <v>923</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.0002419948577880859</v>
       </c>
       <c r="D10">
-        <v>0.6702439024390244</v>
+        <v>0.9004878048780488</v>
       </c>
       <c r="E10">
         <v>1019</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.0006549358367919922</v>
       </c>
       <c r="G10">
         <v>0.9941463414634146</v>

</xml_diff>

<commit_message>
Zeitmessung von verbessert (in ns)
</commit_message>
<xml_diff>
--- a/proj1/outputfiles/output.xlsx
+++ b/proj1/outputfiles/output.xlsx
@@ -454,19 +454,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>120</v>
+        <v>241</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>91200</v>
       </c>
       <c r="D2">
-        <v>40.68</v>
+        <v>81.69</v>
       </c>
       <c r="E2">
         <v>290</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>88200</v>
       </c>
       <c r="G2">
         <v>98.31</v>
@@ -480,19 +480,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>754</v>
+        <v>793</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>149400</v>
       </c>
       <c r="D3">
-        <v>73.63</v>
+        <v>77.44</v>
       </c>
       <c r="E3">
         <v>1018</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>123500</v>
       </c>
       <c r="G3">
         <v>99.41</v>
@@ -506,19 +506,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>62900</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>62.86</v>
       </c>
       <c r="E4">
         <v>35</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>54100</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -535,7 +535,7 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>70200</v>
       </c>
       <c r="D5">
         <v>69.56999999999999</v>
@@ -544,7 +544,7 @@
         <v>16</v>
       </c>
       <c r="F5">
-        <v>0.0009984970092773438</v>
+        <v>51100</v>
       </c>
       <c r="G5">
         <v>69.56999999999999</v>
@@ -558,19 +558,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>72400</v>
       </c>
       <c r="D6">
-        <v>92.31</v>
+        <v>94.23</v>
       </c>
       <c r="E6">
         <v>52</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>74400</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -584,19 +584,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>76500</v>
       </c>
       <c r="D7">
-        <v>86.92</v>
+        <v>39.25</v>
       </c>
       <c r="E7">
         <v>90</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>55800</v>
       </c>
       <c r="G7">
         <v>84.11</v>
@@ -610,19 +610,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>9559</v>
+        <v>9719</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>108500</v>
       </c>
       <c r="D8">
-        <v>97.87</v>
+        <v>99.51000000000001</v>
       </c>
       <c r="E8">
         <v>9753</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>114100</v>
       </c>
       <c r="G8">
         <v>99.86</v>
@@ -636,19 +636,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>64100</v>
       </c>
       <c r="D9">
-        <v>81.54000000000001</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="E9">
         <v>130</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>144800</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -662,19 +662,19 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>738</v>
+        <v>889</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>105800</v>
       </c>
       <c r="D10">
-        <v>72</v>
+        <v>86.73</v>
       </c>
       <c r="E10">
         <v>1019</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>125000</v>
       </c>
       <c r="G10">
         <v>99.41</v>

</xml_diff>

<commit_message>
proj2 zu Projekt hinzugefügt
</commit_message>
<xml_diff>
--- a/proj1/outputfiles/output.xlsx
+++ b/proj1/outputfiles/output.xlsx
@@ -22,7 +22,7 @@
     <t>Results Random</t>
   </si>
   <si>
-    <t>Computing Time (sec)</t>
+    <t>Computing Time (ns)</t>
   </si>
   <si>
     <t>% of Optimum</t>
@@ -454,19 +454,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="C2">
-        <v>91200</v>
+        <v>91600</v>
       </c>
       <c r="D2">
-        <v>81.69</v>
+        <v>69.15000000000001</v>
       </c>
       <c r="E2">
         <v>290</v>
       </c>
       <c r="F2">
-        <v>88200</v>
+        <v>97200</v>
       </c>
       <c r="G2">
         <v>98.31</v>
@@ -480,19 +480,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>793</v>
+        <v>993</v>
       </c>
       <c r="C3">
-        <v>149400</v>
+        <v>109700</v>
       </c>
       <c r="D3">
-        <v>77.44</v>
+        <v>96.97</v>
       </c>
       <c r="E3">
         <v>1018</v>
       </c>
       <c r="F3">
-        <v>123500</v>
+        <v>154300</v>
       </c>
       <c r="G3">
         <v>99.41</v>
@@ -506,19 +506,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C4">
-        <v>62900</v>
+        <v>61300</v>
       </c>
       <c r="D4">
-        <v>62.86</v>
+        <v>94.29000000000001</v>
       </c>
       <c r="E4">
         <v>35</v>
       </c>
       <c r="F4">
-        <v>54100</v>
+        <v>72800</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -535,7 +535,7 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>70200</v>
+        <v>59000</v>
       </c>
       <c r="D5">
         <v>69.56999999999999</v>
@@ -544,7 +544,7 @@
         <v>16</v>
       </c>
       <c r="F5">
-        <v>51100</v>
+        <v>64200</v>
       </c>
       <c r="G5">
         <v>69.56999999999999</v>
@@ -558,19 +558,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6">
-        <v>72400</v>
+        <v>77700</v>
       </c>
       <c r="D6">
-        <v>94.23</v>
+        <v>96.15000000000001</v>
       </c>
       <c r="E6">
         <v>52</v>
       </c>
       <c r="F6">
-        <v>74400</v>
+        <v>86400</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -584,19 +584,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C7">
-        <v>76500</v>
+        <v>62200</v>
       </c>
       <c r="D7">
-        <v>39.25</v>
+        <v>85.05</v>
       </c>
       <c r="E7">
         <v>90</v>
       </c>
       <c r="F7">
-        <v>55800</v>
+        <v>67400</v>
       </c>
       <c r="G7">
         <v>84.11</v>
@@ -610,19 +610,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>9719</v>
+        <v>9738</v>
       </c>
       <c r="C8">
-        <v>108500</v>
+        <v>117900</v>
       </c>
       <c r="D8">
-        <v>99.51000000000001</v>
+        <v>99.7</v>
       </c>
       <c r="E8">
         <v>9753</v>
       </c>
       <c r="F8">
-        <v>114100</v>
+        <v>138200</v>
       </c>
       <c r="G8">
         <v>99.86</v>
@@ -636,19 +636,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9">
-        <v>64100</v>
+        <v>71800</v>
       </c>
       <c r="D9">
-        <v>83.84999999999999</v>
+        <v>81.54000000000001</v>
       </c>
       <c r="E9">
         <v>130</v>
       </c>
       <c r="F9">
-        <v>144800</v>
+        <v>68900</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -662,19 +662,19 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>889</v>
+        <v>788</v>
       </c>
       <c r="C10">
-        <v>105800</v>
+        <v>142400</v>
       </c>
       <c r="D10">
-        <v>86.73</v>
+        <v>76.88</v>
       </c>
       <c r="E10">
         <v>1019</v>
       </c>
       <c r="F10">
-        <v>125000</v>
+        <v>148800</v>
       </c>
       <c r="G10">
         <v>99.41</v>

</xml_diff>

<commit_message>
- demandlist einlesen - random heuristic
</commit_message>
<xml_diff>
--- a/proj1/outputfiles/output.xlsx
+++ b/proj1/outputfiles/output.xlsx
@@ -454,19 +454,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>204</v>
+        <v>166</v>
       </c>
       <c r="C2">
-        <v>91600</v>
+        <v>84100</v>
       </c>
       <c r="D2">
-        <v>69.15000000000001</v>
+        <v>56.27</v>
       </c>
       <c r="E2">
         <v>290</v>
       </c>
       <c r="F2">
-        <v>97200</v>
+        <v>91900</v>
       </c>
       <c r="G2">
         <v>98.31</v>
@@ -480,19 +480,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>993</v>
+        <v>870</v>
       </c>
       <c r="C3">
-        <v>109700</v>
+        <v>104600</v>
       </c>
       <c r="D3">
-        <v>96.97</v>
+        <v>84.95999999999999</v>
       </c>
       <c r="E3">
         <v>1018</v>
       </c>
       <c r="F3">
-        <v>154300</v>
+        <v>147900</v>
       </c>
       <c r="G3">
         <v>99.41</v>
@@ -506,19 +506,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4">
-        <v>61300</v>
+        <v>63900</v>
       </c>
       <c r="D4">
-        <v>94.29000000000001</v>
+        <v>100</v>
       </c>
       <c r="E4">
         <v>35</v>
       </c>
       <c r="F4">
-        <v>72800</v>
+        <v>66400</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -532,19 +532,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>59000</v>
+        <v>61200</v>
       </c>
       <c r="D5">
-        <v>69.56999999999999</v>
+        <v>78.26000000000001</v>
       </c>
       <c r="E5">
         <v>16</v>
       </c>
       <c r="F5">
-        <v>64200</v>
+        <v>62500</v>
       </c>
       <c r="G5">
         <v>69.56999999999999</v>
@@ -558,19 +558,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C6">
-        <v>77700</v>
+        <v>72800</v>
       </c>
       <c r="D6">
-        <v>96.15000000000001</v>
+        <v>78.84999999999999</v>
       </c>
       <c r="E6">
         <v>52</v>
       </c>
       <c r="F6">
-        <v>86400</v>
+        <v>85500</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -584,19 +584,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C7">
-        <v>62200</v>
+        <v>70700</v>
       </c>
       <c r="D7">
-        <v>85.05</v>
+        <v>82.23999999999999</v>
       </c>
       <c r="E7">
         <v>90</v>
       </c>
       <c r="F7">
-        <v>67400</v>
+        <v>64400</v>
       </c>
       <c r="G7">
         <v>84.11</v>
@@ -610,19 +610,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>9738</v>
+        <v>9103</v>
       </c>
       <c r="C8">
-        <v>117900</v>
+        <v>105500</v>
       </c>
       <c r="D8">
-        <v>99.7</v>
+        <v>93.2</v>
       </c>
       <c r="E8">
         <v>9753</v>
       </c>
       <c r="F8">
-        <v>138200</v>
+        <v>133700</v>
       </c>
       <c r="G8">
         <v>99.86</v>
@@ -636,19 +636,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C9">
-        <v>71800</v>
+        <v>59500</v>
       </c>
       <c r="D9">
-        <v>81.54000000000001</v>
+        <v>90.77</v>
       </c>
       <c r="E9">
         <v>130</v>
       </c>
       <c r="F9">
-        <v>68900</v>
+        <v>56100</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -662,19 +662,19 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>788</v>
+        <v>813</v>
       </c>
       <c r="C10">
-        <v>142400</v>
+        <v>95800</v>
       </c>
       <c r="D10">
-        <v>76.88</v>
+        <v>79.31999999999999</v>
       </c>
       <c r="E10">
         <v>1019</v>
       </c>
       <c r="F10">
-        <v>148800</v>
+        <v>123100</v>
       </c>
       <c r="G10">
         <v>99.41</v>

</xml_diff>

<commit_message>
Test Projekt 2 lauffähig
</commit_message>
<xml_diff>
--- a/proj1/outputfiles/output.xlsx
+++ b/proj1/outputfiles/output.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NiklasRuge/PycharmProjects/researchlab_prj1/proj1/outputfiles/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A053DF21-DF4C-0746-8072-2508895785A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -28,7 +22,7 @@
     <t>Results Random</t>
   </si>
   <si>
-    <t>Computing Time (sec)</t>
+    <t>Computing Time (ns)</t>
   </si>
   <si>
     <t>% of Optimum</t>
@@ -97,8 +91,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,23 +125,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -189,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,27 +207,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -273,24 +241,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,22 +416,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,24 +449,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>241</v>
+        <v>159</v>
       </c>
       <c r="C2">
-        <v>91200</v>
+        <v>72900</v>
       </c>
       <c r="D2">
-        <v>81.69</v>
+        <v>53.9</v>
       </c>
       <c r="E2">
         <v>290</v>
       </c>
       <c r="F2">
-        <v>88200</v>
+        <v>82000</v>
       </c>
       <c r="G2">
         <v>98.31</v>
@@ -533,24 +475,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>793</v>
+        <v>851</v>
       </c>
       <c r="C3">
-        <v>149400</v>
+        <v>92700</v>
       </c>
       <c r="D3">
-        <v>77.44</v>
+        <v>83.11</v>
       </c>
       <c r="E3">
         <v>1018</v>
       </c>
       <c r="F3">
-        <v>123500</v>
+        <v>127100</v>
       </c>
       <c r="G3">
         <v>99.41</v>
@@ -559,24 +501,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C4">
-        <v>62900</v>
+        <v>53500</v>
       </c>
       <c r="D4">
-        <v>62.86</v>
+        <v>80</v>
       </c>
       <c r="E4">
         <v>35</v>
       </c>
       <c r="F4">
-        <v>54100</v>
+        <v>56800</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -585,7 +527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -593,42 +535,42 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>70200</v>
+        <v>51500</v>
       </c>
       <c r="D5">
-        <v>69.569999999999993</v>
+        <v>69.56999999999999</v>
       </c>
       <c r="E5">
         <v>16</v>
       </c>
       <c r="F5">
-        <v>51100</v>
+        <v>52500</v>
       </c>
       <c r="G5">
-        <v>69.569999999999993</v>
+        <v>69.56999999999999</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>72400</v>
+        <v>60100</v>
       </c>
       <c r="D6">
-        <v>94.23</v>
+        <v>63.46</v>
       </c>
       <c r="E6">
         <v>52</v>
       </c>
       <c r="F6">
-        <v>74400</v>
+        <v>72000</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -637,24 +579,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C7">
-        <v>76500</v>
+        <v>53400</v>
       </c>
       <c r="D7">
-        <v>39.25</v>
+        <v>65.42</v>
       </c>
       <c r="E7">
         <v>90</v>
       </c>
       <c r="F7">
-        <v>55800</v>
+        <v>55200</v>
       </c>
       <c r="G7">
         <v>84.11</v>
@@ -663,24 +605,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>9719</v>
+        <v>9134</v>
       </c>
       <c r="C8">
-        <v>108500</v>
+        <v>89100</v>
       </c>
       <c r="D8">
-        <v>99.51</v>
+        <v>93.52</v>
       </c>
       <c r="E8">
         <v>9753</v>
       </c>
       <c r="F8">
-        <v>114100</v>
+        <v>113900</v>
       </c>
       <c r="G8">
         <v>99.86</v>
@@ -689,24 +631,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="C9">
-        <v>64100</v>
+        <v>55600</v>
       </c>
       <c r="D9">
-        <v>83.85</v>
+        <v>55.38</v>
       </c>
       <c r="E9">
         <v>130</v>
       </c>
       <c r="F9">
-        <v>144800</v>
+        <v>56200</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -715,24 +657,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>889</v>
+        <v>850</v>
       </c>
       <c r="C10">
-        <v>105800</v>
+        <v>90200</v>
       </c>
       <c r="D10">
-        <v>86.73</v>
+        <v>82.93000000000001</v>
       </c>
       <c r="E10">
         <v>1019</v>
       </c>
       <c r="F10">
-        <v>125000</v>
+        <v>123300</v>
       </c>
       <c r="G10">
         <v>99.41</v>

</xml_diff>